<commit_message>
Updated with REIPPPP included
</commit_message>
<xml_diff>
--- a/data/model_file.xlsx
+++ b/data/model_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3F3BA2-54A7-49EA-82DD-82F177E1F26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417DB235-309E-461B-A771-C51C43465248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">existing_eskom_stations!$A$1:$Y$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">existing_non_eskom_stations!$A$1:$AH$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -554,9 +555,6 @@
     <t>base</t>
   </si>
   <si>
-    <t>landfill</t>
-  </si>
-  <si>
     <t>Droogfontein Solar Power</t>
   </si>
   <si>
@@ -579,6 +577,9 @@
   </si>
   <si>
     <t>solar</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -586,7 +587,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -811,7 +812,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -930,14 +931,17 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1284,8 +1288,8 @@
   <dimension ref="A1:AG81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E66" sqref="E66"/>
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1313,13 +1317,13 @@
         <v>39</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>40</v>
@@ -1328,7 +1332,7 @@
         <v>41</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>55</v>
@@ -1352,7 +1356,7 @@
         <v>71</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q1" s="15" t="s">
         <v>45</v>
@@ -6138,11 +6142,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF5E6A-3574-43A5-9DB4-0F7019EF770D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AH104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J84" sqref="J84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q102" sqref="Q102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6163,21 +6168,21 @@
     <col min="25" max="26" width="15.6328125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="51.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="51" x14ac:dyDescent="0.35">
       <c r="B1" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>178</v>
-      </c>
       <c r="E1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>40</v>
@@ -6186,7 +6191,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>55</v>
@@ -6210,7 +6215,7 @@
         <v>71</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>45</v>
@@ -6240,7 +6245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>170</v>
       </c>
@@ -6251,7 +6256,7 @@
         <v>101</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>2</v>
@@ -6320,7 +6325,7 @@
         <v>21.153960000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>170</v>
       </c>
@@ -6400,7 +6405,7 @@
         <v>25.807017154113002</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>170</v>
       </c>
@@ -6480,7 +6485,7 @@
         <v>19.42878</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
@@ -6491,7 +6496,7 @@
         <v>101</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>2</v>
@@ -6561,7 +6566,7 @@
         <v>24.01981</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>170</v>
       </c>
@@ -6641,7 +6646,7 @@
         <v>26.353794968770501</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>170</v>
       </c>
@@ -6652,7 +6657,7 @@
         <v>101</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>2</v>
@@ -6730,7 +6735,7 @@
       <c r="AG7"/>
       <c r="AH7"/>
     </row>
-    <row r="8" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>170</v>
       </c>
@@ -6741,7 +6746,7 @@
         <v>101</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>2</v>
@@ -6819,7 +6824,7 @@
       <c r="AG8"/>
       <c r="AH8"/>
     </row>
-    <row r="9" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>170</v>
       </c>
@@ -6907,7 +6912,7 @@
       <c r="AG9"/>
       <c r="AH9"/>
     </row>
-    <row r="10" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>170</v>
       </c>
@@ -6918,7 +6923,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>2</v>
@@ -6996,7 +7001,7 @@
       <c r="AG10"/>
       <c r="AH10"/>
     </row>
-    <row r="11" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>170</v>
       </c>
@@ -7084,7 +7089,7 @@
       <c r="AG11"/>
       <c r="AH11"/>
     </row>
-    <row r="12" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>170</v>
       </c>
@@ -7168,7 +7173,7 @@
       <c r="AG12"/>
       <c r="AH12"/>
     </row>
-    <row r="13" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>170</v>
       </c>
@@ -7179,7 +7184,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>2</v>
@@ -7257,7 +7262,7 @@
       <c r="AG13"/>
       <c r="AH13"/>
     </row>
-    <row r="14" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -7345,7 +7350,7 @@
       <c r="AG14"/>
       <c r="AH14"/>
     </row>
-    <row r="15" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>170</v>
       </c>
@@ -7356,7 +7361,7 @@
         <v>101</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>2</v>
@@ -7434,7 +7439,7 @@
       <c r="AG15"/>
       <c r="AH15"/>
     </row>
-    <row r="16" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>170</v>
       </c>
@@ -7445,7 +7450,7 @@
         <v>101</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>2</v>
@@ -7523,7 +7528,7 @@
       <c r="AG16"/>
       <c r="AH16"/>
     </row>
-    <row r="17" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>170</v>
       </c>
@@ -7611,7 +7616,7 @@
       <c r="AG17"/>
       <c r="AH17"/>
     </row>
-    <row r="18" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>170</v>
       </c>
@@ -7622,7 +7627,7 @@
         <v>101</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>2</v>
@@ -7700,7 +7705,7 @@
       <c r="AG18"/>
       <c r="AH18"/>
     </row>
-    <row r="19" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>170</v>
       </c>
@@ -7711,7 +7716,7 @@
         <v>101</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>2</v>
@@ -7789,7 +7794,7 @@
       <c r="AG19"/>
       <c r="AH19"/>
     </row>
-    <row r="20" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>170</v>
       </c>
@@ -7877,7 +7882,7 @@
       <c r="AG20"/>
       <c r="AH20"/>
     </row>
-    <row r="21" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>170</v>
       </c>
@@ -7888,7 +7893,7 @@
         <v>101</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>2</v>
@@ -7966,7 +7971,7 @@
       <c r="AG21"/>
       <c r="AH21"/>
     </row>
-    <row r="22" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>170</v>
       </c>
@@ -7977,7 +7982,7 @@
         <v>101</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>2</v>
@@ -8055,18 +8060,18 @@
       <c r="AG22"/>
       <c r="AH22"/>
     </row>
-    <row r="23" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>170</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" s="35" t="s">
         <v>2</v>
@@ -8144,7 +8149,7 @@
       <c r="AG23"/>
       <c r="AH23"/>
     </row>
-    <row r="24" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>170</v>
       </c>
@@ -8155,7 +8160,7 @@
         <v>101</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" s="38" t="s">
         <v>2</v>
@@ -8233,7 +8238,7 @@
       <c r="AG24"/>
       <c r="AH24"/>
     </row>
-    <row r="25" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>170</v>
       </c>
@@ -8244,7 +8249,7 @@
         <v>101</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>2</v>
@@ -8322,7 +8327,7 @@
       <c r="AG25"/>
       <c r="AH25"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>170</v>
       </c>
@@ -8333,7 +8338,7 @@
         <v>101</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" s="38" t="s">
         <v>2</v>
@@ -8403,7 +8408,7 @@
         <v>29.321799172554801</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>170</v>
       </c>
@@ -8414,7 +8419,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>2</v>
@@ -8484,7 +8489,7 @@
         <v>20.029258108133099</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>170</v>
       </c>
@@ -8564,7 +8569,7 @@
         <v>18.307536545625499</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>170</v>
       </c>
@@ -8575,7 +8580,7 @@
         <v>101</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>2</v>
@@ -8645,7 +8650,7 @@
         <v>29.450761713535101</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>170</v>
       </c>
@@ -8725,7 +8730,7 @@
         <v>26.106440829574002</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>170</v>
       </c>
@@ -8805,7 +8810,7 @@
         <v>17.9958467059943</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>170</v>
       </c>
@@ -8816,7 +8821,7 @@
         <v>102</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>2</v>
@@ -8885,7 +8890,7 @@
         <v>18.4853819813383</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>170</v>
       </c>
@@ -8965,7 +8970,7 @@
         <v>21.919975876760699</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>170</v>
       </c>
@@ -8976,7 +8981,7 @@
         <v>102</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>2</v>
@@ -9045,7 +9050,7 @@
         <v>25.213105911553999</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>170</v>
       </c>
@@ -9125,7 +9130,7 @@
         <v>27.879187501376201</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>170</v>
       </c>
@@ -9136,7 +9141,7 @@
         <v>102</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>2</v>
@@ -9205,7 +9210,7 @@
         <v>26.330198203529498</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>170</v>
       </c>
@@ -9285,7 +9290,7 @@
         <v>19.043998428834399</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>170</v>
       </c>
@@ -9365,7 +9370,7 @@
         <v>25.672221076962899</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>170</v>
       </c>
@@ -9376,7 +9381,7 @@
         <v>102</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E39" s="35" t="s">
         <v>2</v>
@@ -9445,7 +9450,7 @@
         <v>23.104063371285399</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>170</v>
       </c>
@@ -9456,7 +9461,7 @@
         <v>102</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E40" s="38" t="s">
         <v>2</v>
@@ -9525,7 +9530,7 @@
         <v>24.441833856689101</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>170</v>
       </c>
@@ -9605,7 +9610,7 @@
         <v>20.533500298364299</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>170</v>
       </c>
@@ -9616,7 +9621,7 @@
         <v>102</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E42" s="38" t="s">
         <v>2</v>
@@ -9685,7 +9690,7 @@
         <v>23.015895825852599</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>170</v>
       </c>
@@ -9696,7 +9701,7 @@
         <v>102</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E43" s="35" t="s">
         <v>2</v>
@@ -9765,7 +9770,7 @@
         <v>24.01981</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>170</v>
       </c>
@@ -9845,7 +9850,7 @@
         <v>28.4101438223705</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>170</v>
       </c>
@@ -9925,7 +9930,7 @@
         <v>24.344621690645798</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>170</v>
       </c>
@@ -9936,7 +9941,7 @@
         <v>102</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E46" s="38" t="s">
         <v>2</v>
@@ -10005,7 +10010,7 @@
         <v>21.221905297254199</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>170</v>
       </c>
@@ -10016,7 +10021,7 @@
         <v>102</v>
       </c>
       <c r="D47" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E47" s="35" t="s">
         <v>2</v>
@@ -10085,7 +10090,7 @@
         <v>18.516148401131201</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>170</v>
       </c>
@@ -10165,7 +10170,7 @@
         <v>26.5316768686796</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>170</v>
       </c>
@@ -10245,7 +10250,7 @@
         <v>19.386264306318001</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>170</v>
       </c>
@@ -10256,7 +10261,7 @@
         <v>103</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>2</v>
@@ -10336,7 +10341,7 @@
         <v>103</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>171</v>
+        <v>61</v>
       </c>
       <c r="E51" s="35" t="s">
         <v>2</v>
@@ -10405,7 +10410,7 @@
         <v>28.032528400020201</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>170</v>
       </c>
@@ -10485,7 +10490,7 @@
         <v>21.221905297254199</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>170</v>
       </c>
@@ -10565,7 +10570,7 @@
         <v>19.441043457444799</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>170</v>
       </c>
@@ -10645,7 +10650,7 @@
         <v>19.441043457444799</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>170</v>
       </c>
@@ -10725,7 +10730,7 @@
         <v>24.01981</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
         <v>170</v>
       </c>
@@ -10819,7 +10824,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F57" s="35">
         <v>16.5</v>
@@ -10836,14 +10841,14 @@
       <c r="J57" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="K57" s="35">
-        <v>0</v>
+      <c r="K57" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="L57" s="35">
         <v>1650</v>
       </c>
-      <c r="M57" s="35">
-        <v>0</v>
+      <c r="M57" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="N57" s="35" t="s">
         <v>43</v>
@@ -10851,11 +10856,11 @@
       <c r="O57" s="37">
         <v>0</v>
       </c>
-      <c r="P57" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q57" s="35" t="s">
-        <v>43</v>
+      <c r="P57" s="35">
+        <v>1500</v>
+      </c>
+      <c r="Q57" s="35">
+        <v>0</v>
       </c>
       <c r="R57" s="35" t="s">
         <v>43</v>
@@ -10881,7 +10886,7 @@
         <v>32.0345129341963</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>170</v>
       </c>
@@ -10892,7 +10897,7 @@
         <v>103</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E58" s="38" t="s">
         <v>2</v>
@@ -10961,7 +10966,7 @@
         <v>22.339438357413599</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>170</v>
       </c>
@@ -10972,7 +10977,7 @@
         <v>103</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E59" s="35" t="s">
         <v>2</v>
@@ -11041,7 +11046,7 @@
         <v>22.339438357413599</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
         <v>170</v>
       </c>
@@ -11121,7 +11126,7 @@
         <v>25.807017154113002</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>170</v>
       </c>
@@ -11201,7 +11206,7 @@
         <v>24.945973114014201</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
         <v>170</v>
       </c>
@@ -11212,7 +11217,7 @@
         <v>103</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>2</v>
@@ -11281,7 +11286,7 @@
         <v>18.895029014548101</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
         <v>170</v>
       </c>
@@ -11292,7 +11297,7 @@
         <v>103</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E63" s="35" t="s">
         <v>2</v>
@@ -11361,7 +11366,7 @@
         <v>24.798805920214701</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
         <v>170</v>
       </c>
@@ -11441,7 +11446,7 @@
         <v>24.7416286318375</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>170</v>
       </c>
@@ -11452,7 +11457,7 @@
         <v>103</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E65" s="35" t="s">
         <v>2</v>
@@ -11521,7 +11526,7 @@
         <v>27.635734905913498</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
         <v>170</v>
       </c>
@@ -11601,7 +11606,7 @@
         <v>23.015895825852599</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
         <v>170</v>
       </c>
@@ -11681,7 +11686,7 @@
         <v>23.104063371285399</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
         <v>170</v>
       </c>
@@ -11692,7 +11697,7 @@
         <v>104</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E68" s="38" t="s">
         <v>2</v>
@@ -11761,7 +11766,7 @@
         <v>18.915203100908499</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
         <v>170</v>
       </c>
@@ -11772,7 +11777,7 @@
         <v>104</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E69" s="35" t="s">
         <v>2</v>
@@ -11841,7 +11846,7 @@
         <v>23.7490965967927</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
         <v>170</v>
       </c>
@@ -11852,7 +11857,7 @@
         <v>104</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E70" s="38" t="s">
         <v>2</v>
@@ -11921,7 +11926,7 @@
         <v>26.642110714537999</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="8" t="s">
         <v>170</v>
       </c>
@@ -12001,7 +12006,7 @@
         <v>22.339438357413599</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
         <v>170</v>
       </c>
@@ -12012,7 +12017,7 @@
         <v>104</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E72" s="38" t="s">
         <v>2</v>
@@ -12081,7 +12086,7 @@
         <v>27.807654163244202</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="8" t="s">
         <v>170</v>
       </c>
@@ -12092,7 +12097,7 @@
         <v>104</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E73" s="35" t="s">
         <v>2</v>
@@ -12161,7 +12166,7 @@
         <v>21.221905297254199</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="8" t="s">
         <v>170</v>
       </c>
@@ -12172,7 +12177,7 @@
         <v>104</v>
       </c>
       <c r="D74" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E74" s="38" t="s">
         <v>2</v>
@@ -12241,7 +12246,7 @@
         <v>21.221905297254199</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="8" t="s">
         <v>170</v>
       </c>
@@ -12321,7 +12326,7 @@
         <v>20.431854895634601</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
         <v>170</v>
       </c>
@@ -12401,7 +12406,7 @@
         <v>22.339438357413599</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
         <v>170</v>
       </c>
@@ -12481,7 +12486,7 @@
         <v>25.807017154113002</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
         <v>170</v>
       </c>
@@ -12561,7 +12566,7 @@
         <v>17.8877643635381</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="8" t="s">
         <v>170</v>
       </c>
@@ -12572,7 +12577,7 @@
         <v>104</v>
       </c>
       <c r="D79" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E79" s="35" t="s">
         <v>2</v>
@@ -12641,7 +12646,7 @@
         <v>19.386264306318001</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="8" t="s">
         <v>170</v>
       </c>
@@ -12721,7 +12726,7 @@
         <v>28.307683283941302</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="8" t="s">
         <v>170</v>
       </c>
@@ -12732,7 +12737,7 @@
         <v>104</v>
       </c>
       <c r="D81" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E81" s="35" t="s">
         <v>2</v>
@@ -12832,14 +12837,14 @@
       <c r="J82" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="K82" s="38">
-        <v>0</v>
+      <c r="K82" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="L82" s="38">
         <v>1650</v>
       </c>
-      <c r="M82" s="38">
-        <v>0</v>
+      <c r="M82" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="N82" s="38" t="s">
         <v>43</v>
@@ -12847,11 +12852,11 @@
       <c r="O82" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="P82" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q82" s="38" t="s">
-        <v>43</v>
+      <c r="P82" s="38">
+        <v>1500</v>
+      </c>
+      <c r="Q82" s="38">
+        <v>0</v>
       </c>
       <c r="R82" s="38" t="s">
         <v>43</v>
@@ -12877,7 +12882,7 @@
         <v>30.974304836468701</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="8" t="s">
         <v>170</v>
       </c>
@@ -12957,7 +12962,7 @@
         <v>25.807017154113002</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8" t="s">
         <v>170</v>
       </c>
@@ -13037,7 +13042,7 @@
         <v>24.7416286318375</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="8" t="s">
         <v>170</v>
       </c>
@@ -13117,7 +13122,7 @@
         <v>20.029258108133099</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="8" t="s">
         <v>170</v>
       </c>
@@ -13197,7 +13202,7 @@
         <v>20.669836490486698</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="8" t="s">
         <v>170</v>
       </c>
@@ -13208,7 +13213,7 @@
         <v>104</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E87" s="35" t="s">
         <v>2</v>
@@ -13277,7 +13282,7 @@
         <v>21.221905297254199</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8" t="s">
         <v>170</v>
       </c>
@@ -13357,7 +13362,7 @@
         <v>20.669836490486698</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="8" t="s">
         <v>170</v>
       </c>
@@ -13368,7 +13373,7 @@
         <v>104</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E89" s="35" t="s">
         <v>11</v>
@@ -13437,7 +13442,7 @@
         <v>19.441043457444799</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8" t="s">
         <v>170</v>
       </c>
@@ -13517,7 +13522,7 @@
         <v>20.669836490486698</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="8" t="s">
         <v>170</v>
       </c>
@@ -13528,7 +13533,7 @@
         <v>104</v>
       </c>
       <c r="D91" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E91" s="35" t="s">
         <v>2</v>
@@ -13597,7 +13602,7 @@
         <v>24.7048545534144</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="8" t="s">
         <v>170</v>
       </c>
@@ -13677,7 +13682,7 @@
         <v>27.429813102134101</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="8" t="s">
         <v>170</v>
       </c>
@@ -13688,7 +13693,7 @@
         <v>104</v>
       </c>
       <c r="D93" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E93" s="35" t="s">
         <v>2</v>
@@ -13757,7 +13762,7 @@
         <v>26.082419364174601</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="8" t="s">
         <v>170</v>
       </c>
@@ -13765,7 +13770,7 @@
         <v>30</v>
       </c>
       <c r="C94" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D94" s="38" t="s">
         <v>57</v>
@@ -13843,7 +13848,7 @@
       <c r="AG94" s="4"/>
       <c r="AH94" s="4"/>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="8" t="s">
         <v>170</v>
       </c>
@@ -13851,7 +13856,7 @@
         <v>31</v>
       </c>
       <c r="C95" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D95" s="35" t="s">
         <v>57</v>
@@ -13929,7 +13934,7 @@
       <c r="AG95" s="4"/>
       <c r="AH95" s="4"/>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
         <v>170</v>
       </c>
@@ -13937,7 +13942,7 @@
         <v>66</v>
       </c>
       <c r="C96" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D96" s="38" t="s">
         <v>72</v>
@@ -14015,7 +14020,7 @@
       <c r="AG96" s="4"/>
       <c r="AH96" s="4"/>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
         <v>170</v>
       </c>
@@ -14023,7 +14028,7 @@
         <v>67</v>
       </c>
       <c r="C97" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D97" s="35" t="s">
         <v>72</v>
@@ -14101,7 +14106,7 @@
       <c r="AG97" s="4"/>
       <c r="AH97" s="4"/>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
         <v>170</v>
       </c>
@@ -14109,7 +14114,7 @@
         <v>32</v>
       </c>
       <c r="C98" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D98" s="38" t="s">
         <v>63</v>
@@ -14187,7 +14192,7 @@
       <c r="AG98" s="4"/>
       <c r="AH98" s="4"/>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="8" t="s">
         <v>170</v>
       </c>
@@ -14195,7 +14200,7 @@
         <v>33</v>
       </c>
       <c r="C99" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D99" s="35" t="s">
         <v>63</v>
@@ -14273,7 +14278,7 @@
       <c r="AG99" s="4"/>
       <c r="AH99" s="4"/>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="8" t="s">
         <v>170</v>
       </c>
@@ -14281,7 +14286,7 @@
         <v>34</v>
       </c>
       <c r="C100" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D100" s="38" t="s">
         <v>62</v>
@@ -14290,7 +14295,8 @@
         <v>2</v>
       </c>
       <c r="F100" s="38">
-        <v>1500</v>
+        <f>1500*1.176</f>
+        <v>1764</v>
       </c>
       <c r="G100" s="38">
         <v>250</v>
@@ -14355,7 +14361,7 @@
       <c r="AG100" s="4"/>
       <c r="AH100" s="4"/>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="8" t="s">
         <v>170</v>
       </c>
@@ -14363,7 +14369,7 @@
         <v>35</v>
       </c>
       <c r="C101" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D101" s="35" t="s">
         <v>62</v>
@@ -14449,7 +14455,7 @@
         <v>36</v>
       </c>
       <c r="C102" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D102" s="38" t="s">
         <v>61</v>
@@ -14531,7 +14537,7 @@
         <v>37</v>
       </c>
       <c r="C103" s="34" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="D103" s="35" t="s">
         <v>61</v>
@@ -14609,15 +14615,15 @@
       <c r="AG103" s="4"/>
       <c r="AH103" s="4"/>
     </row>
-    <row r="104" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:34" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="28" t="s">
         <v>170</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C104" s="34" t="s">
-        <v>43</v>
+      <c r="C104" s="49" t="s">
+        <v>179</v>
       </c>
       <c r="D104" s="41" t="s">
         <v>60</v>
@@ -14698,6 +14704,13 @@
       <c r="AH104" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AH104" xr:uid="{DECF5E6A-3574-43A5-9DB4-0F7019EF770D}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="biomass"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated topology and base network
</commit_message>
<xml_diff>
--- a/data/model_file.xlsx
+++ b/data/model_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="model_setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -2134,7 +2134,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21800,7 +21800,7 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -23466,7 +23466,7 @@
   <dimension ref="A1:AQ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25462,8 +25462,8 @@
   </sheetPr>
   <dimension ref="A1:L396"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E125" activeCellId="0" sqref="E125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D383" activeCellId="0" sqref="D383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27895,7 +27895,7 @@
       </c>
       <c r="L96" s="123"/>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>14</v>
       </c>
@@ -27931,7 +27931,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="49" t="str">
         <f aca="false">A97</f>
         <v>csir_ambitions_2019</v>
@@ -27968,7 +27968,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="49" t="str">
         <f aca="false">A98</f>
         <v>csir_ambitions_2019</v>
@@ -28005,7 +28005,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="49" t="str">
         <f aca="false">A99</f>
         <v>csir_ambitions_2019</v>
@@ -28042,7 +28042,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="49" t="str">
         <f aca="false">A100</f>
         <v>csir_ambitions_2019</v>
@@ -28077,7 +28077,7 @@
       </c>
       <c r="L101" s="127"/>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="49" t="str">
         <f aca="false">A101</f>
         <v>csir_ambitions_2019</v>
@@ -28114,7 +28114,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="49" t="str">
         <f aca="false">A102</f>
         <v>csir_ambitions_2019</v>
@@ -28188,7 +28188,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="49" t="str">
         <f aca="false">A104</f>
         <v>csir_ambitions_2019</v>
@@ -28225,7 +28225,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="49" t="str">
         <f aca="false">A105</f>
         <v>csir_ambitions_2019</v>
@@ -28262,7 +28262,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="49" t="str">
         <f aca="false">A106</f>
         <v>csir_ambitions_2019</v>
@@ -28299,7 +28299,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="49" t="str">
         <f aca="false">A107</f>
         <v>csir_ambitions_2019</v>
@@ -28336,7 +28336,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="49" t="str">
         <f aca="false">A108</f>
         <v>csir_ambitions_2019</v>
@@ -28373,7 +28373,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="49" t="str">
         <f aca="false">A109</f>
         <v>csir_ambitions_2019</v>
@@ -28410,7 +28410,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="49" t="str">
         <f aca="false">A110</f>
         <v>csir_ambitions_2019</v>
@@ -28447,7 +28447,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="49" t="str">
         <f aca="false">A111</f>
         <v>csir_ambitions_2019</v>
@@ -28484,7 +28484,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="49" t="str">
         <f aca="false">A112</f>
         <v>csir_ambitions_2019</v>
@@ -28521,7 +28521,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="49" t="str">
         <f aca="false">A113</f>
         <v>csir_ambitions_2019</v>
@@ -28558,7 +28558,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="49" t="str">
         <f aca="false">A114</f>
         <v>csir_ambitions_2019</v>
@@ -28640,7 +28640,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="49" t="str">
         <f aca="false">A116</f>
         <v>csir_ambitions_2019</v>
@@ -28679,7 +28679,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="49" t="str">
         <f aca="false">A117</f>
         <v>csir_ambitions_2019</v>
@@ -28718,7 +28718,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="49" t="str">
         <f aca="false">A118</f>
         <v>csir_ambitions_2019</v>
@@ -28757,7 +28757,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="49" t="str">
         <f aca="false">A119</f>
         <v>csir_ambitions_2019</v>
@@ -28796,7 +28796,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="49" t="str">
         <f aca="false">A120</f>
         <v>csir_ambitions_2019</v>
@@ -28835,7 +28835,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="49" t="str">
         <f aca="false">A121</f>
         <v>csir_ambitions_2019</v>
@@ -28874,7 +28874,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="49" t="str">
         <f aca="false">A122</f>
         <v>csir_ambitions_2019</v>
@@ -28913,7 +28913,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="49" t="str">
         <f aca="false">A123</f>
         <v>csir_ambitions_2019</v>
@@ -28952,7 +28952,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="49" t="str">
         <f aca="false">A124</f>
         <v>csir_ambitions_2019</v>
@@ -28991,7 +28991,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="49" t="str">
         <f aca="false">A125</f>
         <v>csir_ambitions_2019</v>
@@ -29030,7 +29030,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="49" t="str">
         <f aca="false">A126</f>
         <v>csir_ambitions_2019</v>
@@ -29067,7 +29067,7 @@
       </c>
       <c r="L127" s="127"/>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="49" t="str">
         <f aca="false">A127</f>
         <v>csir_ambitions_2019</v>
@@ -29106,7 +29106,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="49" t="str">
         <f aca="false">A128</f>
         <v>csir_ambitions_2019</v>
@@ -29145,7 +29145,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="49" t="str">
         <f aca="false">A129</f>
         <v>csir_ambitions_2019</v>
@@ -29184,7 +29184,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="49" t="str">
         <f aca="false">A130</f>
         <v>csir_ambitions_2019</v>
@@ -29223,7 +29223,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="49" t="str">
         <f aca="false">A131</f>
         <v>csir_ambitions_2019</v>
@@ -29267,7 +29267,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="49" t="str">
         <f aca="false">A132</f>
         <v>csir_ambitions_2019</v>
@@ -29311,7 +29311,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="49" t="str">
         <f aca="false">A133</f>
         <v>csir_ambitions_2019</v>
@@ -29355,7 +29355,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="49" t="str">
         <f aca="false">A134</f>
         <v>csir_ambitions_2019</v>
@@ -29380,7 +29380,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="49" t="str">
         <f aca="false">A135</f>
         <v>csir_ambitions_2019</v>
@@ -29419,7 +29419,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="49" t="str">
         <f aca="false">A136</f>
         <v>csir_ambitions_2019</v>
@@ -29458,7 +29458,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="49" t="str">
         <f aca="false">A137</f>
         <v>csir_ambitions_2019</v>
@@ -29497,7 +29497,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="49" t="str">
         <f aca="false">A138</f>
         <v>csir_ambitions_2019</v>
@@ -29536,7 +29536,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="49" t="str">
         <f aca="false">A139</f>
         <v>csir_ambitions_2019</v>
@@ -29575,7 +29575,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="49" t="str">
         <f aca="false">A140</f>
         <v>csir_ambitions_2019</v>
@@ -29637,7 +29637,7 @@
       </c>
       <c r="L142" s="127"/>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="49" t="str">
         <f aca="false">A142</f>
         <v>csir_ambitions_2019</v>
@@ -29674,7 +29674,7 @@
       </c>
       <c r="L143" s="127"/>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="49" t="str">
         <f aca="false">A143</f>
         <v>csir_ambitions_2019</v>
@@ -29711,7 +29711,7 @@
       </c>
       <c r="L144" s="127"/>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="49" t="str">
         <f aca="false">A144</f>
         <v>csir_ambitions_2019</v>
@@ -29748,7 +29748,7 @@
       </c>
       <c r="L145" s="127"/>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="49" t="str">
         <f aca="false">A145</f>
         <v>csir_ambitions_2019</v>
@@ -29785,7 +29785,7 @@
       </c>
       <c r="L146" s="127"/>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="49" t="str">
         <f aca="false">A146</f>
         <v>csir_ambitions_2019</v>
@@ -29808,7 +29808,7 @@
       </c>
       <c r="L147" s="127"/>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="49" t="str">
         <f aca="false">A147</f>
         <v>csir_ambitions_2019</v>
@@ -29845,7 +29845,7 @@
       </c>
       <c r="L148" s="127"/>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="49" t="str">
         <f aca="false">A148</f>
         <v>csir_ambitions_2019</v>
@@ -29882,7 +29882,7 @@
       </c>
       <c r="L149" s="127"/>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="49" t="str">
         <f aca="false">A149</f>
         <v>csir_ambitions_2019</v>
@@ -29905,7 +29905,7 @@
       </c>
       <c r="L150" s="127"/>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="49" t="str">
         <f aca="false">A150</f>
         <v>csir_ambitions_2019</v>
@@ -29942,7 +29942,7 @@
       </c>
       <c r="L151" s="127"/>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="49" t="str">
         <f aca="false">A151</f>
         <v>csir_ambitions_2019</v>
@@ -29965,7 +29965,7 @@
       </c>
       <c r="L152" s="127"/>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="49" t="str">
         <f aca="false">A152</f>
         <v>csir_ambitions_2019</v>
@@ -30002,7 +30002,7 @@
       </c>
       <c r="L153" s="127"/>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="49" t="str">
         <f aca="false">A153</f>
         <v>csir_ambitions_2019</v>
@@ -30039,7 +30039,7 @@
       </c>
       <c r="L154" s="127"/>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="49" t="str">
         <f aca="false">A154</f>
         <v>csir_ambitions_2019</v>
@@ -30076,7 +30076,7 @@
       </c>
       <c r="L155" s="127"/>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="49" t="str">
         <f aca="false">A155</f>
         <v>csir_ambitions_2019</v>
@@ -30113,7 +30113,7 @@
       </c>
       <c r="L156" s="127"/>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="49" t="str">
         <f aca="false">A156</f>
         <v>csir_ambitions_2019</v>
@@ -30150,7 +30150,7 @@
       </c>
       <c r="L157" s="127"/>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="49" t="str">
         <f aca="false">A157</f>
         <v>csir_ambitions_2019</v>
@@ -30187,7 +30187,7 @@
       </c>
       <c r="L158" s="127"/>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="49" t="str">
         <f aca="false">A158</f>
         <v>csir_ambitions_2019</v>
@@ -30224,7 +30224,7 @@
       </c>
       <c r="L159" s="127"/>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="49" t="str">
         <f aca="false">A159</f>
         <v>csir_ambitions_2019</v>
@@ -30267,7 +30267,7 @@
       </c>
       <c r="L160" s="127"/>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="49" t="str">
         <f aca="false">A160</f>
         <v>csir_ambitions_2019</v>
@@ -30350,7 +30350,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="49" t="str">
         <f aca="false">A162</f>
         <v>csir_ambitions_2019</v>
@@ -30390,7 +30390,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="49" t="str">
         <f aca="false">A163</f>
         <v>csir_ambitions_2019</v>
@@ -30418,7 +30418,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="49" t="str">
         <f aca="false">A164</f>
         <v>csir_ambitions_2019</v>
@@ -30458,7 +30458,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="49" t="str">
         <f aca="false">A165</f>
         <v>csir_ambitions_2019</v>
@@ -30498,7 +30498,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="49" t="str">
         <f aca="false">A166</f>
         <v>csir_ambitions_2019</v>
@@ -30538,7 +30538,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="49" t="str">
         <f aca="false">A167</f>
         <v>csir_ambitions_2019</v>
@@ -30563,7 +30563,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="49" t="str">
         <f aca="false">A168</f>
         <v>csir_ambitions_2019</v>
@@ -30603,7 +30603,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="49" t="str">
         <f aca="false">A169</f>
         <v>csir_ambitions_2019</v>
@@ -30643,7 +30643,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="49" t="str">
         <f aca="false">A170</f>
         <v>csir_ambitions_2019</v>
@@ -30683,7 +30683,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="49" t="str">
         <f aca="false">A171</f>
         <v>csir_ambitions_2019</v>
@@ -30723,7 +30723,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="49" t="str">
         <f aca="false">A172</f>
         <v>csir_ambitions_2019</v>
@@ -30763,7 +30763,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="49" t="str">
         <f aca="false">A173</f>
         <v>csir_ambitions_2019</v>
@@ -30803,7 +30803,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="49" t="str">
         <f aca="false">A174</f>
         <v>csir_ambitions_2019</v>
@@ -30843,7 +30843,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="49" t="str">
         <f aca="false">A175</f>
         <v>csir_ambitions_2019</v>
@@ -30883,7 +30883,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="49" t="str">
         <f aca="false">A176</f>
         <v>csir_ambitions_2019</v>
@@ -30923,7 +30923,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="49" t="str">
         <f aca="false">A177</f>
         <v>csir_ambitions_2019</v>
@@ -30963,7 +30963,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="49" t="str">
         <f aca="false">A178</f>
         <v>csir_ambitions_2019</v>
@@ -31003,7 +31003,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="49" t="str">
         <f aca="false">A179</f>
         <v>csir_ambitions_2019</v>
@@ -31043,7 +31043,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="49" t="str">
         <f aca="false">A180</f>
         <v>csir_ambitions_2019</v>
@@ -31083,7 +31083,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="49" t="str">
         <f aca="false">A181</f>
         <v>csir_ambitions_2019</v>
@@ -31123,7 +31123,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="49" t="str">
         <f aca="false">A182</f>
         <v>csir_ambitions_2019</v>
@@ -31163,7 +31163,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="49" t="str">
         <f aca="false">A183</f>
         <v>csir_ambitions_2019</v>
@@ -31203,7 +31203,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="49" t="str">
         <f aca="false">A184</f>
         <v>csir_ambitions_2019</v>
@@ -31243,7 +31243,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="49" t="str">
         <f aca="false">A185</f>
         <v>csir_ambitions_2019</v>
@@ -31283,7 +31283,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="49" t="str">
         <f aca="false">A186</f>
         <v>csir_ambitions_2019</v>
@@ -31323,7 +31323,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="49" t="str">
         <f aca="false">A187</f>
         <v>csir_ambitions_2019</v>
@@ -31363,7 +31363,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="49" t="str">
         <f aca="false">A188</f>
         <v>csir_ambitions_2019</v>
@@ -34990,7 +34990,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="49" t="str">
         <f aca="false">A289</f>
         <v>csir_ambitions_2022</v>
@@ -35434,7 +35434,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="49" t="str">
         <f aca="false">A301</f>
         <v>csir_ambitions_2022</v>
@@ -35445,27 +35445,36 @@
       <c r="C302" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="D302" s="29"/>
-      <c r="E302" s="115" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F302" s="115" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="G302" s="115" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H302" s="115" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="I302" s="115" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="J302" s="115" t="n">
-        <v>2.5</v>
+      <c r="D302" s="128" t="n">
+        <f aca="false">106.5/87.9*D116</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="E302" s="128" t="n">
+        <f aca="false">D302</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="F302" s="128" t="n">
+        <f aca="false">E302</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="G302" s="128" t="n">
+        <f aca="false">F302</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="H302" s="128" t="n">
+        <f aca="false">G302</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="I302" s="128" t="n">
+        <f aca="false">H302</f>
+        <v>917.184300341297</v>
+      </c>
+      <c r="J302" s="128" t="n">
+        <f aca="false">I302</f>
+        <v>917.184300341297</v>
       </c>
       <c r="K302" s="29" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="L302" s="127" t="s">
         <v>260</v>
@@ -36370,7 +36379,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="49" t="str">
         <f aca="false">A327</f>
         <v>csir_ambitions_2022</v>
@@ -37250,7 +37259,7 @@
       </c>
       <c r="L347" s="127"/>
     </row>
-    <row r="348" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="49" t="str">
         <f aca="false">A347</f>
         <v>csir_ambitions_2022</v>
@@ -38423,6 +38432,12 @@
     <filterColumn colId="0">
       <filters>
         <filter val="csir_ambitions_2019"/>
+        <filter val="csir_ambitions_2022"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="battery inverter"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>